<commit_message>
update to view on git
</commit_message>
<xml_diff>
--- a/u-bar-chart.xlsx
+++ b/u-bar-chart.xlsx
@@ -115,13 +115,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
               <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$D$2</c:f>
+              <c:f>Sheet1!$A$2:$E$2</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -139,13 +139,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
               <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$D$3</c:f>
+              <c:f>Sheet1!$A$3:$E$3</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -161,13 +161,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
               <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$D$4</c:f>
+              <c:f>Sheet1!$A$4:$E$4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -183,13 +183,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$D$1</c:f>
+              <c:f>Sheet1!$A$1:$E$1</c:f>
               <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$D$5</c:f>
+              <c:f>Sheet1!$A$5:$E$5</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -343,13 +343,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8798306868850809</v>
+        <v>0.24620924007686884</v>
       </c>
       <c r="C2" t="n">
-        <v>0.399121994845253</v>
+        <v>0.7744770598157588</v>
       </c>
       <c r="D2" t="n">
-        <v>0.23818218385551193</v>
+        <v>0.30300638625243004</v>
       </c>
     </row>
     <row r="3">
@@ -357,13 +357,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7105846224248189</v>
+        <v>0.3630417644531141</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7211880096530945</v>
+        <v>0.2341433777172771</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2716935334674375</v>
+        <v>0.18752857485013474</v>
       </c>
     </row>
     <row r="4">
@@ -371,13 +371,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5510020363962438</v>
+        <v>0.6505125182365086</v>
       </c>
       <c r="C4" t="n">
-        <v>0.34126845885998947</v>
+        <v>0.18576120723450062</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5772945433817903</v>
+        <v>0.22991321372747697</v>
       </c>
     </row>
     <row r="5">
@@ -385,13 +385,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9839188076569014</v>
+        <v>0.30227479120973777</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5163788044478503</v>
+        <v>0.2820220508202078</v>
       </c>
       <c r="D5" t="n">
-        <v>0.031453317877314646</v>
+        <v>0.3588360230309111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>